<commit_message>
Finalizar actualización de variables independientes
</commit_message>
<xml_diff>
--- a/data/Cushing_OK_WTI_Spot_Price_FOB.xlsx
+++ b/data/Cushing_OK_WTI_Spot_Price_FOB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28120"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a98dfaf1ce87dfc/DataScience/Proyectos/time-series-fertilizer-price-predictor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iván Trejo\OneDrive\DataScience\Proyectos\time-series-fertilizer-price-predictor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{72708AF8-914B-451F-AC66-C254550518D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68D15D7B-B6C0-49B9-B579-ACFE0A43DA5A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EE99C1-9675-4BB5-AF7F-9DCEA343EE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{802D6FC4-0862-461F-A561-B52C40D9DA6D}"/>
   </bookViews>
@@ -468,7 +468,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1C8E6F-CFC8-4321-BED1-3C56A220530C}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>